<commit_message>
Add factor for too sick to vote
</commit_message>
<xml_diff>
--- a/PollingPlaceCovidEstimator.xlsx
+++ b/PollingPlaceCovidEstimator.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edstaub/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edstaub/git/pollingPlaceCovidEstimator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85FFF2D0-04C4-FC4D-9BDF-546A557CEDA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A76556-D79E-3449-8540-362F6DBDB168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17220" yWindow="7080" windowWidth="14360" windowHeight="12880" xr2:uid="{1CAC4DC4-20F6-5549-B858-E88DB391A8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Polling place covid case estimator.</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Expected contagious cases at November 2020 polling place</t>
+  </si>
+  <si>
+    <t>Ratio of too-sick-to-vote to contagious voters</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDA1DAC-6CC4-4243-9129-F1147C7315D6}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,58 +537,66 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <f>B7*(1-B13)*B12</f>
-        <v>1500</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <f>B7*(1-B14)*B13*B12</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
-        <f>B6*B11*B14*B10</f>
+      <c r="B19">
+        <f>B6*B11*B15*B10</f>
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:2" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="3">
-        <f>B18*B17/B5</f>
-        <v>8.3333333333333339</v>
+      <c r="B20" s="3">
+        <f>B19*B18/B5</f>
+        <v>4.166666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add link to cdc report
</commit_message>
<xml_diff>
--- a/PollingPlaceCovidEstimator.xlsx
+++ b/PollingPlaceCovidEstimator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edstaub/git/pollingPlaceCovidEstimator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A76556-D79E-3449-8540-362F6DBDB168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547091AE-71FB-C24D-875D-4CC94FBDCF94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="7080" windowWidth="14360" windowHeight="12880" xr2:uid="{1CAC4DC4-20F6-5549-B858-E88DB391A8E5}"/>
+    <workbookView xWindow="10220" yWindow="7080" windowWidth="21360" windowHeight="12880" xr2:uid="{1CAC4DC4-20F6-5549-B858-E88DB391A8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Polling place covid case estimator.</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Ratio of too-sick-to-vote to contagious voters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - see CDC report </t>
   </si>
 </sst>
 </file>
@@ -93,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +127,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -142,16 +153,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDA1DAC-6CC4-4243-9129-F1147C7315D6}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,39 +581,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <f>B7*(1-B14)*B13*B12</f>
         <v>750</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <f>B6*B11*B15*B10</f>
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:2" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3">
-        <f>B19*B18/B5</f>
+      <c r="B21" s="3">
+        <f>B20*B19/B5</f>
         <v>4.166666666666667</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A16" r:id="rId1" xr:uid="{547823DC-AEA5-2248-AF66-75879D12D453}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>